<commit_message>
Individual runs for HPC. Also smaller changes
</commit_message>
<xml_diff>
--- a/Data/Feature_information.xlsx
+++ b/Data/Feature_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarasofiechristiansen/Documents/Clara/DTU/6. semester/Bachelorprojekt/DSB/Kode/Bachelor_project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D435CCB-6828-2E41-A183-D67F576ADA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058677B4-6D92-4040-A49C-2E1386AD9394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="2" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5472" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5464" uniqueCount="437">
   <si>
     <t>Navn</t>
   </si>
@@ -1312,21 +1312,12 @@
     <t>Sickness among DSB locomotive conductors</t>
   </si>
   <si>
-    <t>0 is not holiday, 1 is holiday season</t>
-  </si>
-  <si>
     <t>0 is weekday, 1 is public holiday or weekend</t>
   </si>
   <si>
     <t>Number of changes for DSB train conductors</t>
   </si>
   <si>
-    <t>Seasonality modeled via sinus</t>
-  </si>
-  <si>
-    <t>Seasonality modeled via cosinus</t>
-  </si>
-  <si>
     <t>Number of passengers boarding the train modeled by COWI</t>
   </si>
   <si>
@@ -1361,13 +1352,49 @@
   </si>
   <si>
     <t>Standard deviation of timetable changes made by BaneDanmark</t>
+  </si>
+  <si>
+    <t>inf</t>
+  </si>
+  <si>
+    <t>Timetable changes made by DSB within 72 hours</t>
+  </si>
+  <si>
+    <t>Timetable changes made by DSB total</t>
+  </si>
+  <si>
+    <t>Timetable changes made by DSB within the day</t>
+  </si>
+  <si>
+    <t>Standard deviation of timetable changes made by DSB</t>
+  </si>
+  <si>
+    <t>0 is not holiday, 1 is holiday season (only summer)</t>
+  </si>
+  <si>
+    <t>Number of delays from Sweden in rush hours</t>
+  </si>
+  <si>
+    <t>Number of delays from Sweden in not in rush hours</t>
+  </si>
+  <si>
+    <t>Number of delays from Germany not in rush hours</t>
+  </si>
+  <si>
+    <t>Number of delays from Germany in rush hours</t>
+  </si>
+  <si>
+    <t>Seasonality modeled via sinus function</t>
+  </si>
+  <si>
+    <t>Seasonality modeled via cosinus function</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1498,6 +1525,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1850,12 +1884,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Farve1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7284,8 +7319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8140,10 +8175,10 @@
         <v>402</v>
       </c>
       <c r="C27" t="s">
-        <v>400</v>
-      </c>
-      <c r="D27" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -8172,10 +8207,10 @@
         <v>403</v>
       </c>
       <c r="C28" t="s">
-        <v>400</v>
-      </c>
-      <c r="D28" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
@@ -8204,10 +8239,10 @@
         <v>404</v>
       </c>
       <c r="C29" t="s">
-        <v>400</v>
-      </c>
-      <c r="D29" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -8236,10 +8271,10 @@
         <v>405</v>
       </c>
       <c r="C30" t="s">
-        <v>400</v>
-      </c>
-      <c r="D30" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -8268,10 +8303,10 @@
         <v>406</v>
       </c>
       <c r="C31" t="s">
-        <v>400</v>
-      </c>
-      <c r="D31" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
       </c>
       <c r="E31" t="s">
         <v>11</v>
@@ -8300,10 +8335,10 @@
         <v>407</v>
       </c>
       <c r="C32" t="s">
-        <v>400</v>
-      </c>
-      <c r="D32" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -8329,19 +8364,19 @@
         <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C33" t="s">
-        <v>400</v>
-      </c>
-      <c r="D33" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -8361,19 +8396,19 @@
         <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>411</v>
+        <v>430</v>
       </c>
       <c r="C34" t="s">
-        <v>400</v>
-      </c>
-      <c r="D34" t="s">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -8777,7 +8812,7 @@
         <v>91</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C47" t="s">
         <v>400</v>
@@ -8809,7 +8844,7 @@
         <v>92</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C48" t="s">
         <v>400</v>
@@ -8841,7 +8876,7 @@
         <v>93</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C49" t="s">
         <v>400</v>
@@ -8873,7 +8908,7 @@
         <v>94</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C50" t="s">
         <v>400</v>
@@ -10345,7 +10380,7 @@
         <v>193</v>
       </c>
       <c r="B96" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C96" t="s">
         <v>400</v>
@@ -10376,8 +10411,8 @@
       <c r="A97" t="s">
         <v>194</v>
       </c>
-      <c r="B97" t="s">
-        <v>419</v>
+      <c r="B97" s="4" t="s">
+        <v>416</v>
       </c>
       <c r="C97" t="s">
         <v>400</v>
@@ -10408,8 +10443,8 @@
       <c r="A98" t="s">
         <v>195</v>
       </c>
-      <c r="B98" t="s">
-        <v>400</v>
+      <c r="B98" s="4" t="s">
+        <v>432</v>
       </c>
       <c r="C98" t="s">
         <v>400</v>
@@ -10440,8 +10475,8 @@
       <c r="A99" t="s">
         <v>196</v>
       </c>
-      <c r="B99" t="s">
-        <v>400</v>
+      <c r="B99" s="4" t="s">
+        <v>431</v>
       </c>
       <c r="C99" t="s">
         <v>400</v>
@@ -10472,8 +10507,8 @@
       <c r="A100" t="s">
         <v>197</v>
       </c>
-      <c r="B100" t="s">
-        <v>400</v>
+      <c r="B100" s="5" t="s">
+        <v>433</v>
       </c>
       <c r="C100" t="s">
         <v>400</v>
@@ -10504,8 +10539,8 @@
       <c r="A101" t="s">
         <v>198</v>
       </c>
-      <c r="B101" t="s">
-        <v>400</v>
+      <c r="B101" s="5" t="s">
+        <v>434</v>
       </c>
       <c r="C101" t="s">
         <v>400</v>
@@ -10536,7 +10571,7 @@
       <c r="A102" t="s">
         <v>199</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="4" t="s">
         <v>400</v>
       </c>
       <c r="C102" t="s">
@@ -10568,7 +10603,7 @@
       <c r="A103" t="s">
         <v>202</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="4" t="s">
         <v>400</v>
       </c>
       <c r="C103" t="s">
@@ -10601,7 +10636,7 @@
         <v>205</v>
       </c>
       <c r="B104" t="s">
-        <v>414</v>
+        <v>435</v>
       </c>
       <c r="C104" t="s">
         <v>400</v>
@@ -10633,7 +10668,7 @@
         <v>209</v>
       </c>
       <c r="B105" t="s">
-        <v>415</v>
+        <v>436</v>
       </c>
       <c r="C105" t="s">
         <v>400</v>
@@ -10665,7 +10700,7 @@
         <v>211</v>
       </c>
       <c r="B106" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C106" t="s">
         <v>400</v>
@@ -11081,7 +11116,7 @@
         <v>227</v>
       </c>
       <c r="B119" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C119" t="s">
         <v>400</v>
@@ -11113,7 +11148,7 @@
         <v>228</v>
       </c>
       <c r="B120" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C120" t="s">
         <v>400</v>
@@ -11336,8 +11371,8 @@
       <c r="A127" t="s">
         <v>235</v>
       </c>
-      <c r="B127" t="s">
-        <v>400</v>
+      <c r="B127" s="4" t="s">
+        <v>426</v>
       </c>
       <c r="C127" t="s">
         <v>400</v>
@@ -11369,7 +11404,7 @@
         <v>236</v>
       </c>
       <c r="B128" t="s">
-        <v>400</v>
+        <v>427</v>
       </c>
       <c r="C128" t="s">
         <v>400</v>
@@ -11401,7 +11436,7 @@
         <v>237</v>
       </c>
       <c r="B129" t="s">
-        <v>400</v>
+        <v>428</v>
       </c>
       <c r="C129" t="s">
         <v>400</v>
@@ -11465,7 +11500,7 @@
         <v>239</v>
       </c>
       <c r="B131" t="s">
-        <v>400</v>
+        <v>429</v>
       </c>
       <c r="C131" t="s">
         <v>400</v>
@@ -13734,7 +13769,7 @@
         <v>380</v>
       </c>
       <c r="B202" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C202" t="s">
         <v>400</v>
@@ -13923,7 +13958,7 @@
         <v>391</v>
       </c>
       <c r="B208" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C208" t="s">
         <v>400</v>
@@ -13955,7 +13990,7 @@
         <v>392</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C209" t="s">
         <v>400</v>

</xml_diff>